<commit_message>
I now understand how Alt1 works
</commit_message>
<xml_diff>
--- a/Excel_Challenge_523 - Alphabets Staircase.xlsx
+++ b/Excel_Challenge_523 - Alphabets Staircase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF99061B-E778-46B5-800D-661BDB14B848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52013800-3439-43DD-AF29-5434B09B0A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="28">
   <si>
     <t>R</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -389,60 +395,6 @@
         <a:xfrm>
           <a:off x="3835400" y="3187700"/>
           <a:ext cx="1107440" cy="601131"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>180340</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>48681</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="A close-up of several logos&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC6D15AD-20D5-453E-B22F-1D97B5B3BEC0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3683000" y="3166110"/>
-          <a:ext cx="1069340" cy="597321"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4896,10 +4848,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C06D7A7-61D8-4A38-A371-60FC886B4CB9}">
-  <dimension ref="A2:BA29"/>
+  <dimension ref="A2:BD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BE6" sqref="BE6"/>
+      <selection activeCell="BC8" sqref="BC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4907,7 +4859,7 @@
     <col min="1" max="53" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4915,7 +4867,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BC3" t="s">
+        <v>26</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" t="str" cm="1">
         <f t="array" ref="A4:BA29">_xlfn.MAKEARRAY(B2,2*B2+1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(ABS(2*_xlpm.r-_xlpm.c)&lt;2,CHAR(MOD(_xlpm.r-1,26)+65),"")))</f>
         <v>A</v>
@@ -5076,8 +5036,15 @@
       <c r="BA4" t="str">
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="BC4" cm="1">
+        <f t="array" ref="BC4:BD4">LINEST({1,3,5},{1,2,3},)</f>
+        <v>2</v>
+      </c>
+      <c r="BD4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <v/>
       </c>
@@ -5237,8 +5204,15 @@
       <c r="BA5" t="str">
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="BC5" cm="1">
+        <f t="array" ref="BC5:BD5">LINEST({2,4,6},{1,2,3},)</f>
+        <v>2</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <v/>
       </c>
@@ -5398,8 +5372,15 @@
       <c r="BA6" t="str">
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="BC6" cm="1">
+        <f t="array" ref="BC6:BD6">LINEST({3,5,7},{1,2,3},)</f>
+        <v>2</v>
+      </c>
+      <c r="BD6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <v/>
       </c>
@@ -5560,7 +5541,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <v/>
       </c>
@@ -5721,7 +5702,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <v/>
       </c>
@@ -5882,7 +5863,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <v/>
       </c>
@@ -6043,7 +6024,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <v/>
       </c>
@@ -6204,7 +6185,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <v/>
       </c>
@@ -6365,7 +6346,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <v/>
       </c>
@@ -6526,7 +6507,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <v/>
       </c>
@@ -6687,7 +6668,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <v/>
       </c>
@@ -6848,7 +6829,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <v/>
       </c>
@@ -9105,6 +9086,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>